<commit_message>
Remove excel.php. Bug fixing at assessee controller. Change design at master blade. Add Tax helper and change stock demo excel file at public directory.
</commit_message>
<xml_diff>
--- a/public/export/assessees_list_1.xlsx
+++ b/public/export/assessees_list_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>SL</t>
   </si>
@@ -45,60 +45,6 @@
   </si>
   <si>
     <t>2021-2022</t>
-  </si>
-  <si>
-    <t>A B S SIDDIQUE</t>
-  </si>
-  <si>
-    <t>12/02/2017</t>
-  </si>
-  <si>
-    <t>A K M Fazlul Hoque</t>
-  </si>
-  <si>
-    <t>13/02/2017</t>
-  </si>
-  <si>
-    <t>A K M Mazharul Islam Khan</t>
-  </si>
-  <si>
-    <t>14/02/2018</t>
-  </si>
-  <si>
-    <t>A Latif Khan</t>
-  </si>
-  <si>
-    <t>15/02/2020</t>
-  </si>
-  <si>
-    <t>Joy</t>
-  </si>
-  <si>
-    <t>16/02/2020</t>
-  </si>
-  <si>
-    <t>Araf Karim</t>
-  </si>
-  <si>
-    <t>17/02/2020</t>
-  </si>
-  <si>
-    <t>Shibbir</t>
-  </si>
-  <si>
-    <t>18/02/2020</t>
-  </si>
-  <si>
-    <t>Jayanta Biswas</t>
-  </si>
-  <si>
-    <t>19/02/2020</t>
-  </si>
-  <si>
-    <t>Jabbar</t>
-  </si>
-  <si>
-    <t>20/02/2020</t>
   </si>
 </sst>
 </file>
@@ -437,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,174 +421,6 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>323456789124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>551114329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>323456789125</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>551114330</v>
-      </c>
-      <c r="F3">
-        <v>5000.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>323456789126</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>551114331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>323456789127</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>551114332</v>
-      </c>
-      <c r="F5">
-        <v>1000.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>323456789128</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>551114333</v>
-      </c>
-      <c r="F6">
-        <v>5000.0</v>
-      </c>
-      <c r="H6">
-        <v>1000.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>323456789129</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
-        <v>551114334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>323456789130</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8">
-        <v>551114335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9">
-        <v>323456789131</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9">
-        <v>551114336</v>
-      </c>
-      <c r="G9">
-        <v>5000.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10">
-        <v>323456789132</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10">
-        <v>551114337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>